<commit_message>
completed (d,p) distributions added u ncertainties to spec factors completed first pass occupancies plotted angle dependence of states
</commit_message>
<xml_diff>
--- a/spectroscopic_factors/excel/116Cd_p,d_115Cd_bite_1_spec_factors.xlsx
+++ b/spectroscopic_factors/excel/116Cd_p,d_115Cd_bite_1_spec_factors.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>ENERGY</t>
   </si>
@@ -23,6 +23,9 @@
   </si>
   <si>
     <t>SPECTROSCOPIC_FACTOR</t>
+  </si>
+  <si>
+    <t>ERROR</t>
   </si>
 </sst>
 </file>
@@ -380,13 +383,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D28"/>
+  <dimension ref="A1:E28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:5">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -396,8 +399,11 @@
       <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:4">
+      <c r="E1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -410,8 +416,11 @@
       <c r="D2">
         <v>0.3001581433456334</v>
       </c>
-    </row>
-    <row r="3" spans="1:4">
+      <c r="E2">
+        <v>0.001719006577617426</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -424,8 +433,11 @@
       <c r="D3">
         <v>4.205124776057514</v>
       </c>
-    </row>
-    <row r="4" spans="1:4">
+      <c r="E3">
+        <v>0.05644954807469117</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -438,8 +450,11 @@
       <c r="D4">
         <v>0.5452704116130814</v>
       </c>
-    </row>
-    <row r="5" spans="1:4">
+      <c r="E4">
+        <v>0.006012585757649582</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -452,8 +467,11 @@
       <c r="D5">
         <v>0.01020135940549718</v>
       </c>
-    </row>
-    <row r="6" spans="1:4">
+      <c r="E5">
+        <v>0.0003458087934066839</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -466,8 +484,11 @@
       <c r="D6">
         <v>1.240891900558166</v>
       </c>
-    </row>
-    <row r="7" spans="1:4">
+      <c r="E6">
+        <v>0.009270130991122661</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
       <c r="A7" s="1">
         <v>5</v>
       </c>
@@ -480,8 +501,11 @@
       <c r="D7">
         <v>0.6805997294347251</v>
       </c>
-    </row>
-    <row r="8" spans="1:4">
+      <c r="E7">
+        <v>0.01600016777948418</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
       <c r="A8" s="1">
         <v>6</v>
       </c>
@@ -494,8 +518,11 @@
       <c r="D8">
         <v>0.09209307522994024</v>
       </c>
-    </row>
-    <row r="9" spans="1:4">
+      <c r="E8">
+        <v>0.01339535639708222</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
       <c r="A9" s="1">
         <v>7</v>
       </c>
@@ -508,8 +535,11 @@
       <c r="D9">
         <v>1.309543675683434</v>
       </c>
-    </row>
-    <row r="10" spans="1:4">
+      <c r="E9">
+        <v>0.02022111690960823</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
       <c r="A10" s="1">
         <v>8</v>
       </c>
@@ -522,8 +552,11 @@
       <c r="D10">
         <v>0.2638231725985584</v>
       </c>
-    </row>
-    <row r="11" spans="1:4">
+      <c r="E10">
+        <v>0.004312818147205043</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
       <c r="A11" s="1">
         <v>9</v>
       </c>
@@ -536,8 +569,11 @@
       <c r="D11">
         <v>0.00386414873584542</v>
       </c>
-    </row>
-    <row r="12" spans="1:4">
+      <c r="E11">
+        <v>0.0006779208308500735</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
       <c r="A12" s="1">
         <v>10</v>
       </c>
@@ -550,8 +586,11 @@
       <c r="D12">
         <v>0.2145187684182691</v>
       </c>
-    </row>
-    <row r="13" spans="1:4">
+      <c r="E12">
+        <v>0.01578709551130119</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
       <c r="A13" s="1">
         <v>11</v>
       </c>
@@ -564,8 +603,11 @@
       <c r="D13">
         <v>0.005853848829869612</v>
       </c>
-    </row>
-    <row r="14" spans="1:4">
+      <c r="E13">
+        <v>0.0002906876987435252</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5">
       <c r="A14" s="1">
         <v>12</v>
       </c>
@@ -578,8 +620,11 @@
       <c r="D14">
         <v>0.06307924517240787</v>
       </c>
-    </row>
-    <row r="15" spans="1:4">
+      <c r="E14">
+        <v>0.002605447083208151</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5">
       <c r="A15" s="1">
         <v>13</v>
       </c>
@@ -592,8 +637,11 @@
       <c r="D15">
         <v>0.005099317199715705</v>
       </c>
-    </row>
-    <row r="16" spans="1:4">
+      <c r="E15">
+        <v>0.0002447672255863539</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5">
       <c r="A16" s="1">
         <v>14</v>
       </c>
@@ -606,8 +654,11 @@
       <c r="D16">
         <v>0.4047597126639875</v>
       </c>
-    </row>
-    <row r="17" spans="1:4">
+      <c r="E16">
+        <v>0.00560724076035283</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5">
       <c r="A17" s="1">
         <v>15</v>
       </c>
@@ -620,8 +671,11 @@
       <c r="D17">
         <v>0.06778262424216062</v>
       </c>
-    </row>
-    <row r="18" spans="1:4">
+      <c r="E17">
+        <v>0.002919866890431535</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5">
       <c r="A18" s="1">
         <v>16</v>
       </c>
@@ -634,8 +688,11 @@
       <c r="D18">
         <v>0.132388537820999</v>
       </c>
-    </row>
-    <row r="19" spans="1:4">
+      <c r="E18">
+        <v>0.01265478670347784</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5">
       <c r="A19" s="1">
         <v>17</v>
       </c>
@@ -648,8 +705,11 @@
       <c r="D19">
         <v>0.05599010444281154</v>
       </c>
-    </row>
-    <row r="20" spans="1:4">
+      <c r="E19">
+        <v>0.002419325947724441</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5">
       <c r="A20" s="1">
         <v>18</v>
       </c>
@@ -662,8 +722,11 @@
       <c r="D20">
         <v>0.01073937579287197</v>
       </c>
-    </row>
-    <row r="21" spans="1:4">
+      <c r="E20">
+        <v>0.001271768185997996</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5">
       <c r="A21" s="1">
         <v>19</v>
       </c>
@@ -671,13 +734,16 @@
         <v>901.5034696283052</v>
       </c>
       <c r="C21">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D21">
-        <v>0.05272482613278295</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4">
+        <v>0.02110661336330132</v>
+      </c>
+      <c r="E21">
+        <v>0.002082889476641578</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5">
       <c r="A22" s="1">
         <v>20</v>
       </c>
@@ -690,8 +756,11 @@
       <c r="D22">
         <v>0.007692109490920014</v>
       </c>
-    </row>
-    <row r="23" spans="1:4">
+      <c r="E22">
+        <v>0.0009971253043785204</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5">
       <c r="A23" s="1">
         <v>21</v>
       </c>
@@ -704,8 +773,11 @@
       <c r="D23">
         <v>0.04025515321390195</v>
       </c>
-    </row>
-    <row r="24" spans="1:4">
+      <c r="E23">
+        <v>0.001927108398537859</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5">
       <c r="A24" s="1">
         <v>22</v>
       </c>
@@ -718,8 +790,11 @@
       <c r="D24">
         <v>0.02459555409517391</v>
       </c>
-    </row>
-    <row r="25" spans="1:4">
+      <c r="E24">
+        <v>0.0005541067359372513</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5">
       <c r="A25" s="1">
         <v>23</v>
       </c>
@@ -732,8 +807,11 @@
       <c r="D25">
         <v>0.05025196624348494</v>
       </c>
-    </row>
-    <row r="26" spans="1:4">
+      <c r="E25">
+        <v>0.00546960176799836</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5">
       <c r="A26" s="1">
         <v>24</v>
       </c>
@@ -746,8 +824,11 @@
       <c r="D26">
         <v>0.01446914701747534</v>
       </c>
-    </row>
-    <row r="27" spans="1:4">
+      <c r="E26">
+        <v>0.001101711701838224</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5">
       <c r="A27" s="1">
         <v>25</v>
       </c>
@@ -760,8 +841,11 @@
       <c r="D27">
         <v>0.104462830624382</v>
       </c>
-    </row>
-    <row r="28" spans="1:4">
+      <c r="E27">
+        <v>0.007584759979328066</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5">
       <c r="A28" s="1">
         <v>26</v>
       </c>
@@ -773,6 +857,9 @@
       </c>
       <c r="D28">
         <v>0.3414547701079077</v>
+      </c>
+      <c r="E28">
+        <v>0.005182531202852024</v>
       </c>
     </row>
   </sheetData>

</xml_diff>